<commit_message>
Have simple text field on the page!
</commit_message>
<xml_diff>
--- a/ITimeEntry interface.xlsx
+++ b/ITimeEntry interface.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmzim\Documents\GitHub\TrackMyTime\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A89905ED-AD9C-413E-B5FA-5B5C43FCC69F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6256A5FD-E22E-47C9-B653-BD62C30784E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1A35575C-27AA-4E54-97D3-8F5B93A3E3EF}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="53">
   <si>
     <r>
       <t>export</t>
@@ -2405,8 +2405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3953DD58-B997-4020-B647-D7DEB10ADCE4}">
   <dimension ref="F7:N63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B34" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8:F61"/>
+    <sheetView tabSelected="1" topLeftCell="B31" workbookViewId="0">
+      <selection activeCell="L35" sqref="L35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2938,7 +2938,10 @@
       </c>
       <c r="G40" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>  user: IUser;  //Single person column</v>
+      </c>
+      <c r="K40" t="s">
+        <v>51</v>
       </c>
       <c r="N40" s="2" t="s">
         <v>29</v>
@@ -3092,14 +3095,14 @@
     <row r="50" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F50" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>  timeEntryTBD1?: string;</v>
       </c>
       <c r="G50" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="J50" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="N50" s="2" t="s">
         <v>38</v>
@@ -3108,14 +3111,14 @@
     <row r="51" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F51" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>  timeEntryTBD2?: string;</v>
       </c>
       <c r="G51" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="J51" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="N51" s="2" t="s">
         <v>39</v>
@@ -3124,14 +3127,14 @@
     <row r="52" spans="6:14" x14ac:dyDescent="0.25">
       <c r="F52" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>  timeEntryTBD3?: string;  </v>
       </c>
       <c r="G52" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="J52" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="N52" s="2" t="s">
         <v>40</v>

</xml_diff>

<commit_message>
Have 4 text fields on the page!
</commit_message>
<xml_diff>
--- a/ITimeEntry interface.xlsx
+++ b/ITimeEntry interface.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmzim\Documents\GitHub\TrackMyTime\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6256A5FD-E22E-47C9-B653-BD62C30784E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B50E4744-40D9-4565-8416-3470CCCC5034}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1A35575C-27AA-4E54-97D3-8F5B93A3E3EF}"/>
   </bookViews>
@@ -2403,15 +2403,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3953DD58-B997-4020-B647-D7DEB10ADCE4}">
-  <dimension ref="F7:N63"/>
+  <dimension ref="C7:N63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B31" workbookViewId="0">
-      <selection activeCell="L35" sqref="L35"/>
+      <selection activeCell="C55" sqref="C55:C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="16.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="7" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:14" x14ac:dyDescent="0.25">
       <c r="F7" t="s">
         <v>49</v>
       </c>
@@ -2428,7 +2431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:14" x14ac:dyDescent="0.25">
       <c r="F8" t="str">
         <f>IF(J8="x",N8,"")</f>
         <v>  //Values that would come from Project item</v>
@@ -2447,7 +2450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:14" x14ac:dyDescent="0.25">
       <c r="F9" t="str">
         <f t="shared" ref="F9:F61" si="0">IF(J9="x",N9,"")</f>
         <v/>
@@ -2463,7 +2466,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:14" x14ac:dyDescent="0.25">
       <c r="F10" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2479,7 +2482,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C11" t="str">
+        <f>LEFT(F11,IFERROR(FIND("?",F11)-1, FIND(":",F11)-1)) &amp; "='';"</f>
+        <v>  titleProject='';</v>
+      </c>
       <c r="F11" t="str">
         <f t="shared" si="0"/>
         <v>  titleProject: string;</v>
@@ -2495,7 +2502,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C12" t="str">
+        <f t="shared" ref="C12:C56" si="2">LEFT(F12,IFERROR(FIND("?",F12)-1, FIND(":",F12)-1)) &amp; "='';"</f>
+        <v>  comments='';</v>
+      </c>
       <c r="F12" t="str">
         <f t="shared" si="0"/>
         <v>  comments?: ISmartText;</v>
@@ -2511,7 +2522,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C13" t="str">
+        <f t="shared" si="2"/>
+        <v>  category1='';</v>
+      </c>
       <c r="F13" t="str">
         <f t="shared" si="0"/>
         <v>  category1?: string[];</v>
@@ -2527,7 +2542,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C14" t="str">
+        <f t="shared" si="2"/>
+        <v>  category2='';</v>
+      </c>
       <c r="F14" t="str">
         <f t="shared" si="0"/>
         <v>  category2?: string[];</v>
@@ -2543,7 +2562,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C15" t="str">
+        <f t="shared" si="2"/>
+        <v>  leader='';</v>
+      </c>
       <c r="F15" t="str">
         <f t="shared" si="0"/>
         <v>  leader?: IUser;  //Likely single person column</v>
@@ -2559,7 +2582,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C16" t="str">
+        <f t="shared" si="2"/>
+        <v>  team='';</v>
+      </c>
       <c r="F16" t="str">
         <f t="shared" si="0"/>
         <v>  team?: IUser[];  //Likely multi person column</v>
@@ -2575,7 +2602,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C17" t="str">
+        <f t="shared" si="2"/>
+        <v>  leaderId='';</v>
+      </c>
       <c r="F17" t="str">
         <f t="shared" si="0"/>
         <v>  leaderId?: number;</v>
@@ -2591,7 +2622,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C18" t="str">
+        <f t="shared" si="2"/>
+        <v>  teamIds='';</v>
+      </c>
       <c r="F18" t="str">
         <f t="shared" si="0"/>
         <v>  teamIds?: number[];</v>
@@ -2607,7 +2642,11 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C19" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="F19" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2618,7 +2657,11 @@
       </c>
       <c r="N19" s="3"/>
     </row>
-    <row r="20" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C20" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="F20" t="str">
         <f t="shared" si="0"/>
         <v>  //This block for use in the history list component</v>
@@ -2637,7 +2680,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C21" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="F21" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2653,7 +2700,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C22" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="F22" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2669,7 +2720,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C23" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="F23" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2685,7 +2740,11 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C24" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="F24" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2701,7 +2760,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C25" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="F25" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2717,7 +2780,11 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C26" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="F26" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2728,7 +2795,11 @@
       </c>
       <c r="N26" s="3"/>
     </row>
-    <row r="27" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C27" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="F27" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2744,7 +2815,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C28" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="F28" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2760,7 +2835,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C29" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="F29" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2773,7 +2852,11 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C30" t="str">
+        <f t="shared" si="2"/>
+        <v>  projectID1='';</v>
+      </c>
       <c r="F30" t="str">
         <f t="shared" si="0"/>
         <v>  projectID1?: ISmartText;  //Example Project # - look for strings starting with * and ?</v>
@@ -2789,7 +2872,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C31" t="str">
+        <f t="shared" si="2"/>
+        <v>  projectID2='';</v>
+      </c>
       <c r="F31" t="str">
         <f t="shared" si="0"/>
         <v>  projectID2?: ISmartText;  //Example Cost Center # - look for strings starting with * and ?</v>
@@ -2805,7 +2892,11 @@
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C32" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="F32" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2816,7 +2907,11 @@
       </c>
       <c r="N32" s="3"/>
     </row>
-    <row r="33" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C33" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="F33" t="str">
         <f t="shared" si="0"/>
         <v>  //Values that relate to project list item</v>
@@ -2835,7 +2930,11 @@
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C34" t="str">
+        <f t="shared" si="2"/>
+        <v>  sourceProject='';</v>
+      </c>
       <c r="F34" t="str">
         <f t="shared" si="0"/>
         <v>  sourceProject?: ILink; //Link back to the source project list item.</v>
@@ -2851,7 +2950,11 @@
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C35" t="str">
+        <f t="shared" si="2"/>
+        <v>  activity='';</v>
+      </c>
       <c r="F35" t="str">
         <f t="shared" si="0"/>
         <v>  activity?: ILink; //Link to the activity you worked on</v>
@@ -2867,7 +2970,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C36" t="str">
+        <f t="shared" si="2"/>
+        <v>  ccList='';</v>
+      </c>
       <c r="F36" t="str">
         <f t="shared" si="0"/>
         <v>  ccList?: ILink; //Link to CC List to copy item</v>
@@ -2883,7 +2990,11 @@
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C37" t="str">
+        <f t="shared" si="2"/>
+        <v>  ccEmail='';</v>
+      </c>
       <c r="F37" t="str">
         <f t="shared" si="0"/>
         <v>  ccEmail?: string; //Email to CC List to copy item </v>
@@ -2899,7 +3010,11 @@
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C38" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="F38" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2912,7 +3027,11 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C39" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="F39" t="str">
         <f t="shared" si="0"/>
         <v>  //Values specific to Time Entry</v>
@@ -2931,7 +3050,11 @@
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C40" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="F40" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2947,7 +3070,11 @@
         <v>29</v>
       </c>
     </row>
-    <row r="41" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C41" t="str">
+        <f t="shared" si="2"/>
+        <v>  userId='';</v>
+      </c>
       <c r="F41" t="str">
         <f t="shared" si="0"/>
         <v>  userId: number;</v>
@@ -2963,7 +3090,11 @@
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C42" t="str">
+        <f t="shared" si="2"/>
+        <v>  startTime='';</v>
+      </c>
       <c r="F42" t="str">
         <f t="shared" si="0"/>
         <v>  startTime: any; //Time stamp</v>
@@ -2979,7 +3110,11 @@
         <v>31</v>
       </c>
     </row>
-    <row r="43" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C43" t="str">
+        <f t="shared" si="2"/>
+        <v>  endTime='';</v>
+      </c>
       <c r="F43" t="str">
         <f t="shared" si="0"/>
         <v>  endTime: any; // Time stamp</v>
@@ -2995,7 +3130,11 @@
         <v>32</v>
       </c>
     </row>
-    <row r="44" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C44" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="F44" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3011,7 +3150,11 @@
         <v>33</v>
       </c>
     </row>
-    <row r="45" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C45" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="F45" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3027,7 +3170,11 @@
         <v>34</v>
       </c>
     </row>
-    <row r="46" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C46" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="F46" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3038,7 +3185,11 @@
       </c>
       <c r="N46" s="3"/>
     </row>
-    <row r="47" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C47" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="F47" t="str">
         <f t="shared" si="0"/>
         <v>  //Saves what entry option was used... Since Last, Slider, Manual</v>
@@ -3057,7 +3208,11 @@
         <v>35</v>
       </c>
     </row>
-    <row r="48" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C48" t="str">
+        <f t="shared" si="2"/>
+        <v>  entryType='';</v>
+      </c>
       <c r="F48" t="str">
         <f t="shared" si="0"/>
         <v>  entryType?: string;</v>
@@ -3073,7 +3228,11 @@
         <v>36</v>
       </c>
     </row>
-    <row r="49" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C49" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="F49" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3092,7 +3251,11 @@
         <v>37</v>
       </c>
     </row>
-    <row r="50" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C50" t="str">
+        <f t="shared" si="2"/>
+        <v>  timeEntryTBD1='';</v>
+      </c>
       <c r="F50" t="str">
         <f t="shared" si="0"/>
         <v>  timeEntryTBD1?: string;</v>
@@ -3108,7 +3271,11 @@
         <v>38</v>
       </c>
     </row>
-    <row r="51" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C51" t="str">
+        <f t="shared" si="2"/>
+        <v>  timeEntryTBD2='';</v>
+      </c>
       <c r="F51" t="str">
         <f t="shared" si="0"/>
         <v>  timeEntryTBD2?: string;</v>
@@ -3124,7 +3291,11 @@
         <v>39</v>
       </c>
     </row>
-    <row r="52" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C52" t="str">
+        <f t="shared" si="2"/>
+        <v>  timeEntryTBD3='';</v>
+      </c>
       <c r="F52" t="str">
         <f t="shared" si="0"/>
         <v>  timeEntryTBD3?: string;  </v>
@@ -3140,7 +3311,11 @@
         <v>40</v>
       </c>
     </row>
-    <row r="53" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C53" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="F53" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3151,7 +3326,11 @@
       </c>
       <c r="N53" s="3"/>
     </row>
-    <row r="54" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C54" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="F54" t="str">
         <f t="shared" si="0"/>
         <v>  //Other settings and information</v>
@@ -3170,7 +3349,11 @@
         <v>41</v>
       </c>
     </row>
-    <row r="55" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C55" t="str">
+        <f t="shared" si="2"/>
+        <v>  location='';</v>
+      </c>
       <c r="F55" t="str">
         <f t="shared" si="0"/>
         <v>  location?: string; // Location</v>
@@ -3186,7 +3369,11 @@
         <v>42</v>
       </c>
     </row>
-    <row r="56" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C56" t="str">
+        <f t="shared" si="2"/>
+        <v>  settings='';</v>
+      </c>
       <c r="F56" t="str">
         <f t="shared" si="0"/>
         <v>  settings?: string;</v>
@@ -3202,7 +3389,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="57" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:14" x14ac:dyDescent="0.25">
       <c r="F57" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3213,7 +3400,7 @@
       </c>
       <c r="N57" s="3"/>
     </row>
-    <row r="58" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:14" x14ac:dyDescent="0.25">
       <c r="F58" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3229,7 +3416,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="59" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:14" x14ac:dyDescent="0.25">
       <c r="F59" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3245,7 +3432,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="60" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:14" x14ac:dyDescent="0.25">
       <c r="F60" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3261,7 +3448,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="61" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:14" x14ac:dyDescent="0.25">
       <c r="F61" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -3277,10 +3464,10 @@
         <v>47</v>
       </c>
     </row>
-    <row r="62" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:14" x14ac:dyDescent="0.25">
       <c r="N62" s="3"/>
     </row>
-    <row r="63" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:14" x14ac:dyDescent="0.25">
       <c r="N63" s="2" t="s">
         <v>48</v>
       </c>

</xml_diff>